<commit_message>
updated koper libs files
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/28_Inst_Analysis_Unit_KOPER.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/28_Inst_Analysis_Unit_KOPER.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alberto\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16635" yWindow="0" windowWidth="18315" windowHeight="7380"/>
+    <workbookView xWindow="16638" yWindow="0" windowWidth="18318" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis_Unit" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="306">
   <si>
     <t>Analysis_Unit</t>
   </si>
@@ -927,12 +927,48 @@
   </si>
   <si>
     <t>KOPER_EXPOSURE</t>
+  </si>
+  <si>
+    <t>KOPER_IND_220</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_KOPER_IND_220</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_KOPER_IND_221</t>
+  </si>
+  <si>
+    <t>KOPER_IND_221</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_KOPER_IND_222</t>
+  </si>
+  <si>
+    <t>KOPER_IND_222</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_KOPER_IND_223</t>
+  </si>
+  <si>
+    <t>KOPER_IND_223</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_KOPER_IND_224</t>
+  </si>
+  <si>
+    <t>KOPER_IND_224</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_KOPER_IND_225</t>
+  </si>
+  <si>
+    <t>KOPER_IND_225</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1045,7 +1081,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1093,7 +1135,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2050" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="2050" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1136,7 +1184,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1184,7 +1238,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1232,7 +1292,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1533,23 +1599,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.26171875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.28515625" customWidth="1"/>
-    <col min="9" max="9" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.26171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.26171875" customWidth="1"/>
+    <col min="9" max="9" width="36.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1562,7 +1628,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1591,7 +1657,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1626,21 +1692,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.578125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="3" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="44.578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1650,7 +1716,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1670,7 +1736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1687,7 +1753,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1704,7 +1770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -1721,7 +1787,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1738,7 +1804,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1755,7 +1821,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1772,7 +1838,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1789,7 +1855,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1806,7 +1872,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1823,7 +1889,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1840,7 +1906,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1857,7 +1923,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1874,7 +1940,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1891,7 +1957,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1908,7 +1974,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1925,7 +1991,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1942,7 +2008,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1959,7 +2025,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1976,7 +2042,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1993,7 +2059,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2010,7 +2076,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2027,7 +2093,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2044,7 +2110,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2061,7 +2127,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2078,7 +2144,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
@@ -2095,7 +2161,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4" t="s">
         <v>20</v>
       </c>
@@ -2112,7 +2178,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
@@ -2129,7 +2195,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4" t="s">
         <v>20</v>
       </c>
@@ -2146,7 +2212,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
@@ -2163,7 +2229,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4" t="s">
         <v>20</v>
       </c>
@@ -2180,7 +2246,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="4" t="s">
         <v>20</v>
       </c>
@@ -2197,7 +2263,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="4" t="s">
         <v>20</v>
       </c>
@@ -2214,7 +2280,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="4" t="s">
         <v>20</v>
       </c>
@@ -2231,7 +2297,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
@@ -2248,7 +2314,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4" t="s">
         <v>20</v>
       </c>
@@ -2265,7 +2331,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4" t="s">
         <v>20</v>
       </c>
@@ -2282,7 +2348,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="4" t="s">
         <v>20</v>
       </c>
@@ -2299,7 +2365,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4" t="s">
         <v>20</v>
       </c>
@@ -2316,7 +2382,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="4" t="s">
         <v>20</v>
       </c>
@@ -2333,7 +2399,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="4" t="s">
         <v>20</v>
       </c>
@@ -2350,7 +2416,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="4" t="s">
         <v>20</v>
       </c>
@@ -2367,7 +2433,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="4" t="s">
         <v>20</v>
       </c>
@@ -2384,7 +2450,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="4" t="s">
         <v>20</v>
       </c>
@@ -2401,7 +2467,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4" t="s">
         <v>20</v>
       </c>
@@ -2418,7 +2484,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="4" t="s">
         <v>20</v>
       </c>
@@ -2435,7 +2501,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="4" t="s">
         <v>20</v>
       </c>
@@ -2452,7 +2518,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="4" t="s">
         <v>20</v>
       </c>
@@ -2469,7 +2535,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="4" t="s">
         <v>20</v>
       </c>
@@ -2486,7 +2552,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="4" t="s">
         <v>20</v>
       </c>
@@ -2503,7 +2569,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="4" t="s">
         <v>20</v>
       </c>
@@ -2520,7 +2586,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="4" t="s">
         <v>20</v>
       </c>
@@ -2537,7 +2603,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="4" t="s">
         <v>20</v>
       </c>
@@ -2554,7 +2620,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="4" t="s">
         <v>20</v>
       </c>
@@ -2571,7 +2637,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="4" t="s">
         <v>20</v>
       </c>
@@ -2588,7 +2654,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="4" t="s">
         <v>20</v>
       </c>
@@ -2605,7 +2671,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="4" t="s">
         <v>20</v>
       </c>
@@ -2622,7 +2688,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="4" t="s">
         <v>20</v>
       </c>
@@ -2639,7 +2705,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="4" t="s">
         <v>20</v>
       </c>
@@ -2656,7 +2722,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="4" t="s">
         <v>20</v>
       </c>
@@ -2673,7 +2739,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="4" t="s">
         <v>20</v>
       </c>
@@ -2690,7 +2756,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="4" t="s">
         <v>20</v>
       </c>
@@ -2707,7 +2773,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="4" t="s">
         <v>20</v>
       </c>
@@ -2724,7 +2790,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="4" t="s">
         <v>20</v>
       </c>
@@ -2741,7 +2807,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="4" t="s">
         <v>20</v>
       </c>
@@ -2758,7 +2824,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="4" t="s">
         <v>20</v>
       </c>
@@ -2775,7 +2841,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="4" t="s">
         <v>20</v>
       </c>
@@ -2792,7 +2858,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="4" t="s">
         <v>20</v>
       </c>
@@ -2809,7 +2875,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="4" t="s">
         <v>20</v>
       </c>
@@ -2826,7 +2892,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="4" t="s">
         <v>20</v>
       </c>
@@ -2843,7 +2909,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="4" t="s">
         <v>20</v>
       </c>
@@ -2860,7 +2926,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="4" t="s">
         <v>20</v>
       </c>
@@ -2877,7 +2943,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="4" t="s">
         <v>20</v>
       </c>
@@ -2894,7 +2960,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="4" t="s">
         <v>20</v>
       </c>
@@ -2911,7 +2977,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="4" t="s">
         <v>20</v>
       </c>
@@ -2928,7 +2994,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="4" t="s">
         <v>20</v>
       </c>
@@ -2945,7 +3011,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="4" t="s">
         <v>20</v>
       </c>
@@ -2962,7 +3028,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="4" t="s">
         <v>20</v>
       </c>
@@ -2979,7 +3045,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="4" t="s">
         <v>20</v>
       </c>
@@ -2996,7 +3062,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="4" t="s">
         <v>20</v>
       </c>
@@ -3013,7 +3079,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="4" t="s">
         <v>20</v>
       </c>
@@ -3030,7 +3096,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="4" t="s">
         <v>20</v>
       </c>
@@ -3047,7 +3113,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="4" t="s">
         <v>20</v>
       </c>
@@ -3064,7 +3130,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="4" t="s">
         <v>20</v>
       </c>
@@ -3081,7 +3147,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="4" t="s">
         <v>20</v>
       </c>
@@ -3098,7 +3164,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="4" t="s">
         <v>20</v>
       </c>
@@ -3115,7 +3181,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="4" t="s">
         <v>20</v>
       </c>
@@ -3132,7 +3198,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="4" t="s">
         <v>20</v>
       </c>
@@ -3149,7 +3215,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="4" t="s">
         <v>20</v>
       </c>
@@ -3166,7 +3232,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="4" t="s">
         <v>20</v>
       </c>
@@ -3183,7 +3249,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="4" t="s">
         <v>20</v>
       </c>
@@ -3200,7 +3266,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="4" t="s">
         <v>20</v>
       </c>
@@ -3217,7 +3283,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="4" t="s">
         <v>20</v>
       </c>
@@ -3234,7 +3300,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="4" t="s">
         <v>20</v>
       </c>
@@ -3251,7 +3317,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="4" t="s">
         <v>20</v>
       </c>
@@ -3268,7 +3334,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="4" t="s">
         <v>20</v>
       </c>
@@ -3285,7 +3351,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="4" t="s">
         <v>20</v>
       </c>
@@ -3302,7 +3368,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="4" t="s">
         <v>20</v>
       </c>
@@ -3319,7 +3385,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="4" t="s">
         <v>20</v>
       </c>
@@ -3336,7 +3402,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="4" t="s">
         <v>20</v>
       </c>
@@ -3353,7 +3419,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="4" t="s">
         <v>20</v>
       </c>
@@ -3370,7 +3436,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="4" t="s">
         <v>20</v>
       </c>
@@ -3387,7 +3453,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="4" t="s">
         <v>20</v>
       </c>
@@ -3404,7 +3470,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="4" t="s">
         <v>20</v>
       </c>
@@ -3421,7 +3487,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="4" t="s">
         <v>20</v>
       </c>
@@ -3438,7 +3504,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="4" t="s">
         <v>20</v>
       </c>
@@ -3455,7 +3521,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="4" t="s">
         <v>20</v>
       </c>
@@ -3472,7 +3538,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="4" t="s">
         <v>20</v>
       </c>
@@ -3489,7 +3555,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="4" t="s">
         <v>20</v>
       </c>
@@ -3506,7 +3572,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="4" t="s">
         <v>20</v>
       </c>
@@ -3523,7 +3589,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="4" t="s">
         <v>20</v>
       </c>
@@ -3540,7 +3606,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="4" t="s">
         <v>20</v>
       </c>
@@ -3557,7 +3623,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="4" t="s">
         <v>20</v>
       </c>
@@ -3574,7 +3640,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="4" t="s">
         <v>20</v>
       </c>
@@ -3591,7 +3657,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="4" t="s">
         <v>20</v>
       </c>
@@ -3608,7 +3674,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="4" t="s">
         <v>20</v>
       </c>
@@ -3625,7 +3691,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="4" t="s">
         <v>20</v>
       </c>
@@ -3642,7 +3708,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="4" t="s">
         <v>20</v>
       </c>
@@ -3659,7 +3725,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="4" t="s">
         <v>20</v>
       </c>
@@ -3676,7 +3742,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="4" t="s">
         <v>20</v>
       </c>
@@ -3693,7 +3759,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="4" t="s">
         <v>20</v>
       </c>
@@ -3710,7 +3776,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="4" t="s">
         <v>20</v>
       </c>
@@ -3727,7 +3793,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="4" t="s">
         <v>20</v>
       </c>
@@ -3744,7 +3810,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="4" t="s">
         <v>20</v>
       </c>
@@ -3761,7 +3827,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="4" t="s">
         <v>20</v>
       </c>
@@ -3778,7 +3844,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="4" t="s">
         <v>20</v>
       </c>
@@ -3795,7 +3861,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="4" t="s">
         <v>20</v>
       </c>
@@ -3812,7 +3878,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="4" t="s">
         <v>20</v>
       </c>
@@ -3829,7 +3895,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="4" t="s">
         <v>20</v>
       </c>
@@ -3846,7 +3912,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="4" t="s">
         <v>20</v>
       </c>
@@ -3863,7 +3929,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="4" t="s">
         <v>20</v>
       </c>
@@ -3880,7 +3946,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="4" t="s">
         <v>20</v>
       </c>
@@ -3895,6 +3961,108 @@
       </c>
       <c r="F133" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B134" t="s">
+        <v>295</v>
+      </c>
+      <c r="C134" t="s">
+        <v>295</v>
+      </c>
+      <c r="E134" t="s">
+        <v>26</v>
+      </c>
+      <c r="F134" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B135" t="s">
+        <v>296</v>
+      </c>
+      <c r="C135" t="s">
+        <v>296</v>
+      </c>
+      <c r="E135" t="s">
+        <v>26</v>
+      </c>
+      <c r="F135" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B136" t="s">
+        <v>298</v>
+      </c>
+      <c r="C136" t="s">
+        <v>298</v>
+      </c>
+      <c r="E136" t="s">
+        <v>26</v>
+      </c>
+      <c r="F136" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B137" t="s">
+        <v>300</v>
+      </c>
+      <c r="C137" t="s">
+        <v>300</v>
+      </c>
+      <c r="E137" t="s">
+        <v>26</v>
+      </c>
+      <c r="F137" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B138" t="s">
+        <v>302</v>
+      </c>
+      <c r="C138" t="s">
+        <v>302</v>
+      </c>
+      <c r="E138" t="s">
+        <v>26</v>
+      </c>
+      <c r="F138" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B139" t="s">
+        <v>304</v>
+      </c>
+      <c r="C139" t="s">
+        <v>304</v>
+      </c>
+      <c r="E139" t="s">
+        <v>26</v>
+      </c>
+      <c r="F139" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -3910,18 +4078,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.26171875" customWidth="1"/>
+    <col min="2" max="3" width="19.578125" customWidth="1"/>
+    <col min="4" max="4" width="13.68359375" customWidth="1"/>
+    <col min="5" max="7" width="11.68359375" customWidth="1"/>
+    <col min="8" max="8" width="19.578125" customWidth="1"/>
     <col min="9" max="9" width="39" customWidth="1"/>
-    <col min="10" max="13" width="11.7109375" customWidth="1"/>
+    <col min="10" max="13" width="11.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -3956,7 +4124,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="12.9" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -3991,7 +4159,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>